<commit_message>
finish dev of alliance shrine
</commit_message>
<xml_diff>
--- a/gameData/shared/AllianceShrine.xlsx
+++ b/gameData/shared/AllianceShrine.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7580" yWindow="3100" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="7220" yWindow="3540" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="shrineStage" sheetId="4" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="59">
   <si>
     <t>INT_suggestPlayer</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -164,177 +164,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>a:1,b:1,c:1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>a:2,b:2,c:2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>a:3,b:3,c:3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>a:4,b:4,c:4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>a:1,b:1,c:2</t>
-  </si>
-  <si>
-    <t>a:2,b:2,c:3</t>
-  </si>
-  <si>
-    <t>a:3,b:3,c:4</t>
-  </si>
-  <si>
-    <t>a:1,b:1,c:3</t>
-  </si>
-  <si>
-    <t>a:2,b:2,c:4</t>
-  </si>
-  <si>
-    <t>a:3,b:3,c:5</t>
-  </si>
-  <si>
-    <t>a:2,b:2,c:5</t>
-  </si>
-  <si>
-    <t>a:3,b:3,c:6</t>
-  </si>
-  <si>
-    <t>a:2,b:2,c:6</t>
-  </si>
-  <si>
-    <t>a:3,b:3,c:7</t>
-  </si>
-  <si>
-    <t>a:2,b:2,c:7</t>
-  </si>
-  <si>
-    <t>a:3,b:3,c:8</t>
-  </si>
-  <si>
-    <t>a:2,b:2,c:8</t>
-  </si>
-  <si>
-    <t>a:3,b:3,c:9</t>
-  </si>
-  <si>
-    <t>a:2,b:2,c:9</t>
-  </si>
-  <si>
-    <t>a:3,b:3,c:10</t>
-  </si>
-  <si>
-    <t>a:2,b:2,c:10</t>
-  </si>
-  <si>
-    <t>a:3,b:3,c:11</t>
-  </si>
-  <si>
-    <t>a:2,b:2,c:11</t>
-  </si>
-  <si>
-    <t>a:3,b:3,c:12</t>
-  </si>
-  <si>
-    <t>a:2,b:2,c:12</t>
-  </si>
-  <si>
-    <t>a:3,b:3,c:13</t>
-  </si>
-  <si>
-    <t>a:2,b:2,c:13</t>
-  </si>
-  <si>
-    <t>a:3,b:3,c:14</t>
-  </si>
-  <si>
-    <t>a:2,b:2,c:14</t>
-  </si>
-  <si>
-    <t>a:3,b:3,c:15</t>
-  </si>
-  <si>
-    <t>a:2,b:2,c:15</t>
-  </si>
-  <si>
-    <t>a:3,b:3,c:16</t>
-  </si>
-  <si>
-    <t>a:2,b:2,c:16</t>
-  </si>
-  <si>
-    <t>a:3,b:3,c:17</t>
-  </si>
-  <si>
-    <t>a:4,b:4,c:5</t>
-  </si>
-  <si>
-    <t>a:4,b:4,c:6</t>
-  </si>
-  <si>
-    <t>a:4,b:4,c:7</t>
-  </si>
-  <si>
-    <t>a:4,b:4,c:8</t>
-  </si>
-  <si>
-    <t>a:4,b:4,c:9</t>
-  </si>
-  <si>
-    <t>a:4,b:4,c:10</t>
-  </si>
-  <si>
-    <t>a:4,b:4,c:11</t>
-  </si>
-  <si>
-    <t>a:4,b:4,c:12</t>
-  </si>
-  <si>
-    <t>a:4,b:4,c:13</t>
-  </si>
-  <si>
-    <t>a:4,b:4,c:14</t>
-  </si>
-  <si>
-    <t>a:4,b:4,c:15</t>
-  </si>
-  <si>
-    <t>a:4,b:4,c:16</t>
-  </si>
-  <si>
-    <t>a:4,b:4,c:17</t>
-  </si>
-  <si>
-    <t>a:4,b:4,c:18</t>
-  </si>
-  <si>
-    <t>a:1,b:1,c:4</t>
-  </si>
-  <si>
-    <t>a:1,b:1,c:5</t>
-  </si>
-  <si>
-    <t>a:1,b:1,c:6</t>
-  </si>
-  <si>
-    <t>a:1,b:1,c:7</t>
-  </si>
-  <si>
-    <t>a:1,b:1,c:8</t>
-  </si>
-  <si>
     <t>STR_troops</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>INT_star2DeathPopulation</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>swordsman_1:10,sentinel_1:10,ranger_1:10&amp;swordsman_1:10,sentinel_1:10,ranger_1:10</t>
   </si>
   <si>
@@ -388,6 +221,17 @@
   </si>
   <si>
     <t>swordsman_1:10,sentinel_1:10,ranger_1:10&amp;swordsman_1:10,sentinel_1:10,ranger_1:10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a:b:1,b:c:1,c:d:1</t>
+  </si>
+  <si>
+    <t>a:b:1,b:c:1,c:d:1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT_star2DeathCitizen</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -474,8 +318,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="123">
+  <cellStyleXfs count="127">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -608,7 +456,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="123">
+  <cellStyles count="127">
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
@@ -670,6 +518,8 @@
     <cellStyle name="超链接" xfId="117" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="119" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="125" builtinId="8" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
@@ -731,6 +581,8 @@
     <cellStyle name="访问过的超链接" xfId="118" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="120" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="126" builtinId="9" hidden="1"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1062,8 +914,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R31"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -1098,10 +950,10 @@
         <v>1</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>92</v>
+        <v>39</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>93</v>
+        <v>58</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>37</v>
@@ -1110,25 +962,25 @@
         <v>38</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>102</v>
+        <v>48</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>104</v>
+        <v>50</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>106</v>
+        <v>52</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>103</v>
+        <v>49</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>105</v>
+        <v>51</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>107</v>
+        <v>53</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>108</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="15">
@@ -1154,7 +1006,7 @@
         <v>350</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>109</v>
+        <v>55</v>
       </c>
       <c r="I2" s="2">
         <v>50</v>
@@ -1169,22 +1021,22 @@
         <v>200</v>
       </c>
       <c r="M2" s="2">
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="N2" s="2">
-        <v>150</v>
+        <v>10</v>
       </c>
       <c r="O2" s="2">
-        <v>200</v>
+        <v>20</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="15">
@@ -1210,7 +1062,7 @@
         <v>400</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>95</v>
+        <v>41</v>
       </c>
       <c r="I3" s="2">
         <v>100</v>
@@ -1234,13 +1086,13 @@
         <v>300</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="15">
@@ -1266,7 +1118,7 @@
         <v>450</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>96</v>
+        <v>42</v>
       </c>
       <c r="I4" s="2">
         <v>150</v>
@@ -1290,13 +1142,13 @@
         <v>400</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="15">
@@ -1322,7 +1174,7 @@
         <v>500</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>97</v>
+        <v>43</v>
       </c>
       <c r="I5" s="2">
         <v>200</v>
@@ -1346,13 +1198,13 @@
         <v>500</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="15">
@@ -1378,7 +1230,7 @@
         <v>1000</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>98</v>
+        <v>44</v>
       </c>
       <c r="I6" s="2">
         <v>250</v>
@@ -1402,13 +1254,13 @@
         <v>600</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="15">
@@ -1434,7 +1286,7 @@
         <v>2000</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>99</v>
+        <v>45</v>
       </c>
       <c r="I7" s="2">
         <v>300</v>
@@ -1458,13 +1310,13 @@
         <v>700</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="15">
@@ -1490,7 +1342,7 @@
         <v>2500</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>100</v>
+        <v>46</v>
       </c>
       <c r="I8" s="2">
         <v>350</v>
@@ -1514,13 +1366,13 @@
         <v>800</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="R8" s="2" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="15">
@@ -1546,7 +1398,7 @@
         <v>3000</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>101</v>
+        <v>47</v>
       </c>
       <c r="I9" s="2">
         <v>400</v>
@@ -1570,13 +1422,13 @@
         <v>900</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="R9" s="2" t="s">
-        <v>75</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="15">
@@ -1602,7 +1454,7 @@
         <v>3500</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>101</v>
+        <v>47</v>
       </c>
       <c r="I10" s="2">
         <v>450</v>
@@ -1626,13 +1478,13 @@
         <v>1000</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="R10" s="2" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="15">
@@ -1658,7 +1510,7 @@
         <v>4000</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>101</v>
+        <v>47</v>
       </c>
       <c r="I11" s="2">
         <v>500</v>
@@ -1682,13 +1534,13 @@
         <v>1100</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="Q11" s="2" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="R11" s="2" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="15">
@@ -1714,7 +1566,7 @@
         <v>5000</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>94</v>
+        <v>40</v>
       </c>
       <c r="I12" s="2">
         <v>550</v>
@@ -1738,13 +1590,13 @@
         <v>1200</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="R12" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="15">
@@ -1770,7 +1622,7 @@
         <v>6000</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>94</v>
+        <v>40</v>
       </c>
       <c r="I13" s="2">
         <v>600</v>
@@ -1794,13 +1646,13 @@
         <v>1300</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
       <c r="Q13" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="R13" s="2" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:18" ht="15">
@@ -1826,7 +1678,7 @@
         <v>7000</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>94</v>
+        <v>40</v>
       </c>
       <c r="I14" s="2">
         <v>650</v>
@@ -1850,10 +1702,10 @@
         <v>1400</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>87</v>
+        <v>56</v>
       </c>
       <c r="Q14" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="R14" s="2" t="s">
         <v>56</v>
@@ -1882,7 +1734,7 @@
         <v>8000</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>94</v>
+        <v>40</v>
       </c>
       <c r="I15" s="2">
         <v>700</v>
@@ -1906,13 +1758,13 @@
         <v>1500</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="Q15" s="2" t="s">
         <v>56</v>
       </c>
       <c r="R15" s="2" t="s">
-        <v>78</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:18" ht="15">
@@ -1938,7 +1790,7 @@
         <v>10000</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>94</v>
+        <v>40</v>
       </c>
       <c r="I16" s="2">
         <v>750</v>
@@ -1962,13 +1814,13 @@
         <v>1600</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="Q16" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="R16" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:18" ht="15">
@@ -1994,7 +1846,7 @@
         <v>15000</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>94</v>
+        <v>40</v>
       </c>
       <c r="I17" s="2">
         <v>800</v>
@@ -2018,13 +1870,13 @@
         <v>1700</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>75</v>
+        <v>56</v>
       </c>
       <c r="Q17" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="R17" s="2" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:18" ht="15">
@@ -2050,7 +1902,7 @@
         <v>20000</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>94</v>
+        <v>40</v>
       </c>
       <c r="I18" s="2">
         <v>850</v>
@@ -2074,13 +1926,13 @@
         <v>1800</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>88</v>
+        <v>56</v>
       </c>
       <c r="Q18" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="R18" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:18" ht="15">
@@ -2106,7 +1958,7 @@
         <v>25000</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>94</v>
+        <v>40</v>
       </c>
       <c r="I19" s="2">
         <v>900</v>
@@ -2130,13 +1982,13 @@
         <v>1900</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="Q19" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="R19" s="2" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:18" ht="15">
@@ -2162,7 +2014,7 @@
         <v>30000</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>94</v>
+        <v>40</v>
       </c>
       <c r="I20" s="2">
         <v>950</v>
@@ -2186,13 +2038,13 @@
         <v>2000</v>
       </c>
       <c r="P20" s="2" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="Q20" s="2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="R20" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:18" ht="15">
@@ -2218,7 +2070,7 @@
         <v>35000</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>94</v>
+        <v>40</v>
       </c>
       <c r="I21" s="2">
         <v>1000</v>
@@ -2242,13 +2094,13 @@
         <v>2100</v>
       </c>
       <c r="P21" s="2" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="Q21" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="R21" s="2" t="s">
-        <v>81</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:18" ht="15">
@@ -2274,7 +2126,7 @@
         <v>50000</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>94</v>
+        <v>40</v>
       </c>
       <c r="I22" s="2">
         <v>1050</v>
@@ -2298,13 +2150,13 @@
         <v>2200</v>
       </c>
       <c r="P22" s="2" t="s">
-        <v>89</v>
+        <v>56</v>
       </c>
       <c r="Q22" s="2" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="R22" s="2" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:18" ht="15">
@@ -2330,7 +2182,7 @@
         <v>55000</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>94</v>
+        <v>40</v>
       </c>
       <c r="I23" s="2">
         <v>1100</v>
@@ -2354,13 +2206,13 @@
         <v>2300</v>
       </c>
       <c r="P23" s="2" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="Q23" s="2" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="R23" s="2" t="s">
-        <v>82</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:18" ht="20" customHeight="1">
@@ -2386,7 +2238,7 @@
         <v>60000</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>94</v>
+        <v>40</v>
       </c>
       <c r="I24" s="2">
         <v>1150</v>
@@ -2410,13 +2262,13 @@
         <v>2400</v>
       </c>
       <c r="P24" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="Q24" s="2" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="R24" s="2" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:18" ht="20" customHeight="1">
@@ -2442,7 +2294,7 @@
         <v>65000</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>94</v>
+        <v>40</v>
       </c>
       <c r="I25" s="2">
         <v>1200</v>
@@ -2466,13 +2318,13 @@
         <v>2500</v>
       </c>
       <c r="P25" s="2" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="Q25" s="2" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="R25" s="2" t="s">
-        <v>83</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:18" ht="20" customHeight="1">
@@ -2498,7 +2350,7 @@
         <v>70000</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>94</v>
+        <v>40</v>
       </c>
       <c r="I26" s="2">
         <v>1250</v>
@@ -2522,13 +2374,13 @@
         <v>2600</v>
       </c>
       <c r="P26" s="2" t="s">
-        <v>90</v>
+        <v>56</v>
       </c>
       <c r="Q26" s="2" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="R26" s="2" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:18" ht="20" customHeight="1">
@@ -2554,7 +2406,7 @@
         <v>100000</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>94</v>
+        <v>40</v>
       </c>
       <c r="I27" s="2">
         <v>1300</v>
@@ -2578,13 +2430,13 @@
         <v>2700</v>
       </c>
       <c r="P27" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="Q27" s="2" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="R27" s="2" t="s">
-        <v>84</v>
+        <v>56</v>
       </c>
     </row>
     <row r="28" spans="1:18" ht="20" customHeight="1">
@@ -2610,7 +2462,7 @@
         <v>150000</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>94</v>
+        <v>40</v>
       </c>
       <c r="I28" s="2">
         <v>1350</v>
@@ -2637,10 +2489,10 @@
         <v>56</v>
       </c>
       <c r="Q28" s="2" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="R28" s="2" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
     </row>
     <row r="29" spans="1:18" ht="20" customHeight="1">
@@ -2666,7 +2518,7 @@
         <v>200000</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>94</v>
+        <v>40</v>
       </c>
       <c r="I29" s="2">
         <v>1400</v>
@@ -2690,13 +2542,13 @@
         <v>2900</v>
       </c>
       <c r="P29" s="2" t="s">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="Q29" s="2" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="R29" s="2" t="s">
-        <v>85</v>
+        <v>56</v>
       </c>
     </row>
     <row r="30" spans="1:18" ht="20" customHeight="1">
@@ -2722,7 +2574,7 @@
         <v>250000</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>94</v>
+        <v>40</v>
       </c>
       <c r="I30" s="2">
         <v>1450</v>
@@ -2746,13 +2598,13 @@
         <v>3000</v>
       </c>
       <c r="P30" s="2" t="s">
-        <v>91</v>
+        <v>56</v>
       </c>
       <c r="Q30" s="2" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="R30" s="2" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
     </row>
     <row r="31" spans="1:18" ht="20" customHeight="1">
@@ -2778,7 +2630,7 @@
         <v>300000</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>94</v>
+        <v>40</v>
       </c>
       <c r="I31" s="2">
         <v>1500</v>
@@ -2802,13 +2654,13 @@
         <v>3100</v>
       </c>
       <c r="P31" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Q31" s="2" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="R31" s="2" t="s">
-        <v>86</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bugfix for alliance shrine
</commit_message>
<xml_diff>
--- a/gameData/shared/AllianceShrine.xlsx
+++ b/gameData/shared/AllianceShrine.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7220" yWindow="3540" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="7460" yWindow="1780" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="shrineStage" sheetId="4" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="60">
   <si>
     <t>INT_suggestPlayer</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -233,6 +233,10 @@
   <si>
     <t>INT_star2DeathCitizen</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT_index</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -318,8 +322,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="127">
+  <cellStyleXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -456,7 +462,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="127">
+  <cellStyles count="129">
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
@@ -520,6 +526,7 @@
     <cellStyle name="超链接" xfId="121" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="123" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="127" builtinId="8" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
@@ -583,6 +590,7 @@
     <cellStyle name="访问过的超链接" xfId="122" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="124" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="128" builtinId="9" hidden="1"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -912,78 +920,81 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R31"/>
+  <dimension ref="A1:S31"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="4" width="20.6640625" style="2"/>
-    <col min="5" max="6" width="24.1640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="21.1640625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="33" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="20.6640625" style="2"/>
+    <col min="1" max="5" width="20.6640625" style="2"/>
+    <col min="6" max="7" width="24.1640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="21.1640625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="33" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="20.6640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="1" customFormat="1" ht="15">
+    <row r="1" spans="1:19" s="1" customFormat="1" ht="15">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="15">
+    <row r="2" spans="1:19" ht="15">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -994,43 +1005,43 @@
         <v>1</v>
       </c>
       <c r="D2" s="2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2">
         <v>1000</v>
       </c>
-      <c r="E2" s="2">
+      <c r="F2" s="2">
         <v>50</v>
       </c>
-      <c r="F2" s="2">
+      <c r="G2" s="2">
         <v>3</v>
       </c>
-      <c r="G2" s="2">
+      <c r="H2" s="2">
         <v>350</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="I2" s="2">
+      <c r="J2" s="2">
         <v>50</v>
       </c>
-      <c r="J2" s="2">
+      <c r="K2" s="2">
         <v>100</v>
       </c>
-      <c r="K2" s="2">
+      <c r="L2" s="2">
         <v>150</v>
       </c>
-      <c r="L2" s="2">
+      <c r="M2" s="2">
         <v>200</v>
       </c>
-      <c r="M2" s="2">
+      <c r="N2" s="2">
         <v>5</v>
       </c>
-      <c r="N2" s="2">
+      <c r="O2" s="2">
         <v>10</v>
       </c>
-      <c r="O2" s="2">
+      <c r="P2" s="2">
         <v>20</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>57</v>
       </c>
       <c r="Q2" s="2" t="s">
         <v>57</v>
@@ -1038,55 +1049,58 @@
       <c r="R2" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" ht="15">
+      <c r="S2" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="15">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="2">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2">
         <v>1</v>
       </c>
-      <c r="C3" s="2">
+      <c r="D3" s="2">
         <v>2</v>
       </c>
-      <c r="D3" s="2">
+      <c r="E3" s="2">
         <v>2000</v>
       </c>
-      <c r="E3" s="2">
+      <c r="F3" s="2">
         <v>60</v>
       </c>
-      <c r="F3" s="2">
+      <c r="G3" s="2">
         <v>5</v>
       </c>
-      <c r="G3" s="2">
+      <c r="H3" s="2">
         <v>400</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="I3" s="2">
+      <c r="J3" s="2">
         <v>100</v>
       </c>
-      <c r="J3" s="2">
+      <c r="K3" s="2">
         <v>150</v>
       </c>
-      <c r="K3" s="2">
+      <c r="L3" s="2">
         <v>200</v>
       </c>
-      <c r="L3" s="2">
+      <c r="M3" s="2">
         <v>250</v>
       </c>
-      <c r="M3" s="2">
+      <c r="N3" s="2">
         <v>200</v>
       </c>
-      <c r="N3" s="2">
+      <c r="O3" s="2">
         <v>250</v>
       </c>
-      <c r="O3" s="2">
+      <c r="P3" s="2">
         <v>300</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>57</v>
       </c>
       <c r="Q3" s="2" t="s">
         <v>57</v>
@@ -1094,55 +1108,58 @@
       <c r="R3" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" ht="15">
+      <c r="S3" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="15">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="2">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2">
         <v>1</v>
       </c>
-      <c r="C4" s="2">
+      <c r="D4" s="2">
         <v>3</v>
       </c>
-      <c r="D4" s="2">
+      <c r="E4" s="2">
         <v>3000</v>
       </c>
-      <c r="E4" s="2">
+      <c r="F4" s="2">
         <v>70</v>
       </c>
-      <c r="F4" s="2">
+      <c r="G4" s="2">
         <v>8</v>
       </c>
-      <c r="G4" s="2">
+      <c r="H4" s="2">
         <v>450</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="I4" s="2">
+      <c r="J4" s="2">
         <v>150</v>
       </c>
-      <c r="J4" s="2">
+      <c r="K4" s="2">
         <v>200</v>
       </c>
-      <c r="K4" s="2">
+      <c r="L4" s="2">
         <v>250</v>
-      </c>
-      <c r="L4" s="2">
-        <v>300</v>
       </c>
       <c r="M4" s="2">
         <v>300</v>
       </c>
       <c r="N4" s="2">
+        <v>300</v>
+      </c>
+      <c r="O4" s="2">
         <v>350</v>
       </c>
-      <c r="O4" s="2">
+      <c r="P4" s="2">
         <v>400</v>
-      </c>
-      <c r="P4" s="2" t="s">
-        <v>57</v>
       </c>
       <c r="Q4" s="2" t="s">
         <v>57</v>
@@ -1150,1516 +1167,1600 @@
       <c r="R4" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" ht="15">
+      <c r="S4" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="15">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="2">
+        <v>4</v>
+      </c>
+      <c r="C5" s="2">
         <v>1</v>
       </c>
-      <c r="C5" s="2">
+      <c r="D5" s="2">
         <v>4</v>
       </c>
-      <c r="D5" s="2">
+      <c r="E5" s="2">
         <v>4000</v>
       </c>
-      <c r="E5" s="2">
+      <c r="F5" s="2">
         <v>80</v>
       </c>
-      <c r="F5" s="2">
+      <c r="G5" s="2">
         <v>10</v>
       </c>
-      <c r="G5" s="2">
+      <c r="H5" s="2">
         <v>500</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="I5" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="I5" s="2">
+      <c r="J5" s="2">
         <v>200</v>
       </c>
-      <c r="J5" s="2">
+      <c r="K5" s="2">
         <v>250</v>
       </c>
-      <c r="K5" s="2">
+      <c r="L5" s="2">
         <v>300</v>
       </c>
-      <c r="L5" s="2">
+      <c r="M5" s="2">
         <v>350</v>
       </c>
-      <c r="M5" s="2">
+      <c r="N5" s="2">
         <v>400</v>
       </c>
-      <c r="N5" s="2">
+      <c r="O5" s="2">
         <v>450</v>
       </c>
-      <c r="O5" s="2">
+      <c r="P5" s="2">
         <v>500</v>
       </c>
-      <c r="P5" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="Q5" s="2" t="s">
         <v>56</v>
       </c>
       <c r="R5" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" ht="15">
+      <c r="S5" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="15">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="2">
+        <v>5</v>
+      </c>
+      <c r="C6" s="2">
         <v>1</v>
       </c>
-      <c r="C6" s="2">
+      <c r="D6" s="2">
         <v>5</v>
       </c>
-      <c r="D6" s="2">
+      <c r="E6" s="2">
         <v>5000</v>
       </c>
-      <c r="E6" s="2">
+      <c r="F6" s="2">
         <v>90</v>
       </c>
-      <c r="F6" s="2">
+      <c r="G6" s="2">
         <v>11</v>
       </c>
-      <c r="G6" s="2">
+      <c r="H6" s="2">
         <v>1000</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="I6" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="I6" s="2">
+      <c r="J6" s="2">
         <v>250</v>
       </c>
-      <c r="J6" s="2">
+      <c r="K6" s="2">
         <v>300</v>
       </c>
-      <c r="K6" s="2">
+      <c r="L6" s="2">
         <v>350</v>
       </c>
-      <c r="L6" s="2">
+      <c r="M6" s="2">
         <v>400</v>
       </c>
-      <c r="M6" s="2">
+      <c r="N6" s="2">
         <v>500</v>
       </c>
-      <c r="N6" s="2">
+      <c r="O6" s="2">
         <v>550</v>
       </c>
-      <c r="O6" s="2">
+      <c r="P6" s="2">
         <v>600</v>
       </c>
-      <c r="P6" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="Q6" s="2" t="s">
         <v>56</v>
       </c>
       <c r="R6" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" ht="15">
+      <c r="S6" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="15">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="2">
+        <v>6</v>
+      </c>
+      <c r="C7" s="2">
         <v>2</v>
       </c>
-      <c r="C7" s="2">
+      <c r="D7" s="2">
         <v>1</v>
       </c>
-      <c r="D7" s="2">
+      <c r="E7" s="2">
         <v>6000</v>
       </c>
-      <c r="E7" s="2">
+      <c r="F7" s="2">
         <v>100</v>
       </c>
-      <c r="F7" s="2">
+      <c r="G7" s="2">
         <v>12</v>
       </c>
-      <c r="G7" s="2">
+      <c r="H7" s="2">
         <v>2000</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="I7" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="I7" s="2">
+      <c r="J7" s="2">
         <v>300</v>
       </c>
-      <c r="J7" s="2">
+      <c r="K7" s="2">
         <v>350</v>
       </c>
-      <c r="K7" s="2">
+      <c r="L7" s="2">
         <v>400</v>
       </c>
-      <c r="L7" s="2">
+      <c r="M7" s="2">
         <v>450</v>
       </c>
-      <c r="M7" s="2">
+      <c r="N7" s="2">
         <v>600</v>
       </c>
-      <c r="N7" s="2">
+      <c r="O7" s="2">
         <v>650</v>
       </c>
-      <c r="O7" s="2">
+      <c r="P7" s="2">
         <v>700</v>
       </c>
-      <c r="P7" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="Q7" s="2" t="s">
         <v>56</v>
       </c>
       <c r="R7" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" ht="15">
+      <c r="S7" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="15">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="2">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C8" s="2">
         <v>2</v>
       </c>
       <c r="D8" s="2">
+        <v>2</v>
+      </c>
+      <c r="E8" s="2">
         <v>7000</v>
       </c>
-      <c r="E8" s="2">
+      <c r="F8" s="2">
         <v>110</v>
       </c>
-      <c r="F8" s="2">
+      <c r="G8" s="2">
         <v>13</v>
       </c>
-      <c r="G8" s="2">
+      <c r="H8" s="2">
         <v>2500</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="I8" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I8" s="2">
+      <c r="J8" s="2">
         <v>350</v>
       </c>
-      <c r="J8" s="2">
+      <c r="K8" s="2">
         <v>400</v>
       </c>
-      <c r="K8" s="2">
+      <c r="L8" s="2">
         <v>450</v>
       </c>
-      <c r="L8" s="2">
+      <c r="M8" s="2">
         <v>500</v>
       </c>
-      <c r="M8" s="2">
+      <c r="N8" s="2">
         <v>700</v>
       </c>
-      <c r="N8" s="2">
+      <c r="O8" s="2">
         <v>750</v>
       </c>
-      <c r="O8" s="2">
+      <c r="P8" s="2">
         <v>800</v>
       </c>
-      <c r="P8" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="Q8" s="2" t="s">
         <v>56</v>
       </c>
       <c r="R8" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" ht="15">
+      <c r="S8" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="15">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="2">
+        <v>8</v>
+      </c>
+      <c r="C9" s="2">
         <v>2</v>
       </c>
-      <c r="C9" s="2">
+      <c r="D9" s="2">
         <v>3</v>
       </c>
-      <c r="D9" s="2">
+      <c r="E9" s="2">
         <v>8000</v>
       </c>
-      <c r="E9" s="2">
+      <c r="F9" s="2">
         <v>120</v>
       </c>
-      <c r="F9" s="2">
+      <c r="G9" s="2">
         <v>14</v>
       </c>
-      <c r="G9" s="2">
+      <c r="H9" s="2">
         <v>3000</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="I9" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="I9" s="2">
+      <c r="J9" s="2">
         <v>400</v>
       </c>
-      <c r="J9" s="2">
+      <c r="K9" s="2">
         <v>450</v>
       </c>
-      <c r="K9" s="2">
+      <c r="L9" s="2">
         <v>500</v>
       </c>
-      <c r="L9" s="2">
+      <c r="M9" s="2">
         <v>550</v>
       </c>
-      <c r="M9" s="2">
+      <c r="N9" s="2">
         <v>800</v>
       </c>
-      <c r="N9" s="2">
+      <c r="O9" s="2">
         <v>850</v>
       </c>
-      <c r="O9" s="2">
+      <c r="P9" s="2">
         <v>900</v>
       </c>
-      <c r="P9" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="Q9" s="2" t="s">
         <v>56</v>
       </c>
       <c r="R9" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="10" spans="1:18" ht="15">
+      <c r="S9" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="15">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B10" s="2">
+        <v>9</v>
+      </c>
+      <c r="C10" s="2">
         <v>2</v>
       </c>
-      <c r="C10" s="2">
+      <c r="D10" s="2">
         <v>4</v>
       </c>
-      <c r="D10" s="2">
+      <c r="E10" s="2">
         <v>9000</v>
       </c>
-      <c r="E10" s="2">
+      <c r="F10" s="2">
         <v>130</v>
       </c>
-      <c r="F10" s="2">
+      <c r="G10" s="2">
         <v>15</v>
       </c>
-      <c r="G10" s="2">
+      <c r="H10" s="2">
         <v>3500</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="I10" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="I10" s="2">
+      <c r="J10" s="2">
         <v>450</v>
       </c>
-      <c r="J10" s="2">
+      <c r="K10" s="2">
         <v>500</v>
       </c>
-      <c r="K10" s="2">
+      <c r="L10" s="2">
         <v>550</v>
       </c>
-      <c r="L10" s="2">
+      <c r="M10" s="2">
         <v>600</v>
       </c>
-      <c r="M10" s="2">
+      <c r="N10" s="2">
         <v>900</v>
       </c>
-      <c r="N10" s="2">
+      <c r="O10" s="2">
         <v>950</v>
       </c>
-      <c r="O10" s="2">
+      <c r="P10" s="2">
         <v>1000</v>
       </c>
-      <c r="P10" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="Q10" s="2" t="s">
         <v>56</v>
       </c>
       <c r="R10" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="11" spans="1:18" ht="15">
+      <c r="S10" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="15">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B11" s="2">
+        <v>10</v>
+      </c>
+      <c r="C11" s="2">
         <v>2</v>
       </c>
-      <c r="C11" s="2">
+      <c r="D11" s="2">
         <v>5</v>
       </c>
-      <c r="D11" s="2">
+      <c r="E11" s="2">
         <v>10000</v>
       </c>
-      <c r="E11" s="2">
+      <c r="F11" s="2">
         <v>140</v>
       </c>
-      <c r="F11" s="2">
+      <c r="G11" s="2">
         <v>16</v>
       </c>
-      <c r="G11" s="2">
+      <c r="H11" s="2">
         <v>4000</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="I11" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="I11" s="2">
+      <c r="J11" s="2">
         <v>500</v>
       </c>
-      <c r="J11" s="2">
+      <c r="K11" s="2">
         <v>550</v>
       </c>
-      <c r="K11" s="2">
+      <c r="L11" s="2">
         <v>600</v>
       </c>
-      <c r="L11" s="2">
+      <c r="M11" s="2">
         <v>650</v>
       </c>
-      <c r="M11" s="2">
+      <c r="N11" s="2">
         <v>1000</v>
       </c>
-      <c r="N11" s="2">
+      <c r="O11" s="2">
         <v>1050</v>
       </c>
-      <c r="O11" s="2">
+      <c r="P11" s="2">
         <v>1100</v>
       </c>
-      <c r="P11" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="Q11" s="2" t="s">
         <v>56</v>
       </c>
       <c r="R11" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="12" spans="1:18" ht="15">
+      <c r="S11" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="15">
       <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B12" s="2">
+        <v>11</v>
+      </c>
+      <c r="C12" s="2">
         <v>3</v>
       </c>
-      <c r="C12" s="2">
+      <c r="D12" s="2">
         <v>1</v>
       </c>
-      <c r="D12" s="2">
+      <c r="E12" s="2">
         <v>11000</v>
       </c>
-      <c r="E12" s="2">
+      <c r="F12" s="2">
         <v>150</v>
       </c>
-      <c r="F12" s="2">
+      <c r="G12" s="2">
         <v>17</v>
       </c>
-      <c r="G12" s="2">
+      <c r="H12" s="2">
         <v>5000</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="I12" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I12" s="2">
+      <c r="J12" s="2">
         <v>550</v>
       </c>
-      <c r="J12" s="2">
+      <c r="K12" s="2">
         <v>600</v>
       </c>
-      <c r="K12" s="2">
+      <c r="L12" s="2">
         <v>650</v>
       </c>
-      <c r="L12" s="2">
+      <c r="M12" s="2">
         <v>700</v>
       </c>
-      <c r="M12" s="2">
+      <c r="N12" s="2">
         <v>1100</v>
       </c>
-      <c r="N12" s="2">
+      <c r="O12" s="2">
         <v>1150</v>
       </c>
-      <c r="O12" s="2">
+      <c r="P12" s="2">
         <v>1200</v>
       </c>
-      <c r="P12" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="Q12" s="2" t="s">
         <v>56</v>
       </c>
       <c r="R12" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="13" spans="1:18" ht="15">
+      <c r="S12" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" ht="15">
       <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B13" s="2">
+        <v>12</v>
+      </c>
+      <c r="C13" s="2">
         <v>3</v>
       </c>
-      <c r="C13" s="2">
+      <c r="D13" s="2">
         <v>2</v>
       </c>
-      <c r="D13" s="2">
+      <c r="E13" s="2">
         <v>12000</v>
       </c>
-      <c r="E13" s="2">
+      <c r="F13" s="2">
         <v>160</v>
       </c>
-      <c r="F13" s="2">
+      <c r="G13" s="2">
         <v>18</v>
       </c>
-      <c r="G13" s="2">
+      <c r="H13" s="2">
         <v>6000</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="I13" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I13" s="2">
+      <c r="J13" s="2">
         <v>600</v>
       </c>
-      <c r="J13" s="2">
+      <c r="K13" s="2">
         <v>650</v>
       </c>
-      <c r="K13" s="2">
+      <c r="L13" s="2">
         <v>700</v>
       </c>
-      <c r="L13" s="2">
+      <c r="M13" s="2">
         <v>750</v>
       </c>
-      <c r="M13" s="2">
+      <c r="N13" s="2">
         <v>1200</v>
       </c>
-      <c r="N13" s="2">
+      <c r="O13" s="2">
         <v>1250</v>
       </c>
-      <c r="O13" s="2">
+      <c r="P13" s="2">
         <v>1300</v>
       </c>
-      <c r="P13" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="Q13" s="2" t="s">
         <v>56</v>
       </c>
       <c r="R13" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="14" spans="1:18" ht="15">
+      <c r="S13" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" ht="15">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="2">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C14" s="2">
         <v>3</v>
       </c>
       <c r="D14" s="2">
+        <v>3</v>
+      </c>
+      <c r="E14" s="2">
         <v>13000</v>
       </c>
-      <c r="E14" s="2">
+      <c r="F14" s="2">
         <v>170</v>
       </c>
-      <c r="F14" s="2">
+      <c r="G14" s="2">
         <v>19</v>
       </c>
-      <c r="G14" s="2">
+      <c r="H14" s="2">
         <v>7000</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="I14" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I14" s="2">
+      <c r="J14" s="2">
         <v>650</v>
       </c>
-      <c r="J14" s="2">
+      <c r="K14" s="2">
         <v>700</v>
       </c>
-      <c r="K14" s="2">
+      <c r="L14" s="2">
         <v>750</v>
       </c>
-      <c r="L14" s="2">
+      <c r="M14" s="2">
         <v>800</v>
       </c>
-      <c r="M14" s="2">
+      <c r="N14" s="2">
         <v>1300</v>
       </c>
-      <c r="N14" s="2">
+      <c r="O14" s="2">
         <v>1350</v>
       </c>
-      <c r="O14" s="2">
+      <c r="P14" s="2">
         <v>1400</v>
       </c>
-      <c r="P14" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="Q14" s="2" t="s">
         <v>56</v>
       </c>
       <c r="R14" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="15" spans="1:18" ht="15">
+      <c r="S14" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" ht="15">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B15" s="2">
+        <v>14</v>
+      </c>
+      <c r="C15" s="2">
         <v>3</v>
       </c>
-      <c r="C15" s="2">
+      <c r="D15" s="2">
         <v>4</v>
       </c>
-      <c r="D15" s="2">
+      <c r="E15" s="2">
         <v>14000</v>
       </c>
-      <c r="E15" s="2">
+      <c r="F15" s="2">
         <v>180</v>
       </c>
-      <c r="F15" s="2">
+      <c r="G15" s="2">
         <v>20</v>
       </c>
-      <c r="G15" s="2">
+      <c r="H15" s="2">
         <v>8000</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="I15" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I15" s="2">
+      <c r="J15" s="2">
         <v>700</v>
       </c>
-      <c r="J15" s="2">
+      <c r="K15" s="2">
         <v>750</v>
       </c>
-      <c r="K15" s="2">
+      <c r="L15" s="2">
         <v>800</v>
       </c>
-      <c r="L15" s="2">
+      <c r="M15" s="2">
         <v>850</v>
       </c>
-      <c r="M15" s="2">
+      <c r="N15" s="2">
         <v>1400</v>
       </c>
-      <c r="N15" s="2">
+      <c r="O15" s="2">
         <v>1450</v>
       </c>
-      <c r="O15" s="2">
+      <c r="P15" s="2">
         <v>1500</v>
       </c>
-      <c r="P15" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="Q15" s="2" t="s">
         <v>56</v>
       </c>
       <c r="R15" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="16" spans="1:18" ht="15">
+      <c r="S15" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" ht="15">
       <c r="A16" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B16" s="2">
+        <v>15</v>
+      </c>
+      <c r="C16" s="2">
         <v>3</v>
       </c>
-      <c r="C16" s="2">
+      <c r="D16" s="2">
         <v>5</v>
       </c>
-      <c r="D16" s="2">
+      <c r="E16" s="2">
         <v>15000</v>
       </c>
-      <c r="E16" s="2">
+      <c r="F16" s="2">
         <v>190</v>
       </c>
-      <c r="F16" s="2">
+      <c r="G16" s="2">
         <v>21</v>
       </c>
-      <c r="G16" s="2">
+      <c r="H16" s="2">
         <v>10000</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="I16" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I16" s="2">
+      <c r="J16" s="2">
         <v>750</v>
       </c>
-      <c r="J16" s="2">
+      <c r="K16" s="2">
         <v>800</v>
       </c>
-      <c r="K16" s="2">
+      <c r="L16" s="2">
         <v>850</v>
       </c>
-      <c r="L16" s="2">
+      <c r="M16" s="2">
         <v>900</v>
       </c>
-      <c r="M16" s="2">
+      <c r="N16" s="2">
         <v>1500</v>
       </c>
-      <c r="N16" s="2">
+      <c r="O16" s="2">
         <v>1550</v>
       </c>
-      <c r="O16" s="2">
+      <c r="P16" s="2">
         <v>1600</v>
       </c>
-      <c r="P16" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="Q16" s="2" t="s">
         <v>56</v>
       </c>
       <c r="R16" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="17" spans="1:18" ht="15">
+      <c r="S16" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" ht="15">
       <c r="A17" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B17" s="2">
+        <v>16</v>
+      </c>
+      <c r="C17" s="2">
         <v>4</v>
       </c>
-      <c r="C17" s="2">
+      <c r="D17" s="2">
         <v>1</v>
       </c>
-      <c r="D17" s="2">
+      <c r="E17" s="2">
         <v>16000</v>
       </c>
-      <c r="E17" s="2">
+      <c r="F17" s="2">
         <v>200</v>
       </c>
-      <c r="F17" s="2">
+      <c r="G17" s="2">
         <v>22</v>
       </c>
-      <c r="G17" s="2">
+      <c r="H17" s="2">
         <v>15000</v>
       </c>
-      <c r="H17" s="2" t="s">
+      <c r="I17" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I17" s="2">
+      <c r="J17" s="2">
         <v>800</v>
       </c>
-      <c r="J17" s="2">
+      <c r="K17" s="2">
         <v>850</v>
       </c>
-      <c r="K17" s="2">
+      <c r="L17" s="2">
         <v>900</v>
       </c>
-      <c r="L17" s="2">
+      <c r="M17" s="2">
         <v>950</v>
       </c>
-      <c r="M17" s="2">
+      <c r="N17" s="2">
         <v>1600</v>
       </c>
-      <c r="N17" s="2">
+      <c r="O17" s="2">
         <v>1650</v>
       </c>
-      <c r="O17" s="2">
+      <c r="P17" s="2">
         <v>1700</v>
       </c>
-      <c r="P17" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="Q17" s="2" t="s">
         <v>56</v>
       </c>
       <c r="R17" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="18" spans="1:18" ht="15">
+      <c r="S17" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" ht="15">
       <c r="A18" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B18" s="2">
+        <v>17</v>
+      </c>
+      <c r="C18" s="2">
         <v>4</v>
       </c>
-      <c r="C18" s="2">
+      <c r="D18" s="2">
         <v>2</v>
       </c>
-      <c r="D18" s="2">
+      <c r="E18" s="2">
         <v>17000</v>
       </c>
-      <c r="E18" s="2">
+      <c r="F18" s="2">
         <v>210</v>
       </c>
-      <c r="F18" s="2">
+      <c r="G18" s="2">
         <v>23</v>
       </c>
-      <c r="G18" s="2">
+      <c r="H18" s="2">
         <v>20000</v>
       </c>
-      <c r="H18" s="2" t="s">
+      <c r="I18" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I18" s="2">
+      <c r="J18" s="2">
         <v>850</v>
       </c>
-      <c r="J18" s="2">
+      <c r="K18" s="2">
         <v>900</v>
       </c>
-      <c r="K18" s="2">
+      <c r="L18" s="2">
         <v>950</v>
       </c>
-      <c r="L18" s="2">
+      <c r="M18" s="2">
         <v>1000</v>
       </c>
-      <c r="M18" s="2">
+      <c r="N18" s="2">
         <v>1700</v>
       </c>
-      <c r="N18" s="2">
+      <c r="O18" s="2">
         <v>1750</v>
       </c>
-      <c r="O18" s="2">
+      <c r="P18" s="2">
         <v>1800</v>
       </c>
-      <c r="P18" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="Q18" s="2" t="s">
         <v>56</v>
       </c>
       <c r="R18" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="19" spans="1:18" ht="15">
+      <c r="S18" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" ht="15">
       <c r="A19" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B19" s="2">
+        <v>18</v>
+      </c>
+      <c r="C19" s="2">
         <v>4</v>
       </c>
-      <c r="C19" s="2">
+      <c r="D19" s="2">
         <v>3</v>
       </c>
-      <c r="D19" s="2">
+      <c r="E19" s="2">
         <v>18000</v>
       </c>
-      <c r="E19" s="2">
+      <c r="F19" s="2">
         <v>220</v>
       </c>
-      <c r="F19" s="2">
+      <c r="G19" s="2">
         <v>24</v>
       </c>
-      <c r="G19" s="2">
+      <c r="H19" s="2">
         <v>25000</v>
       </c>
-      <c r="H19" s="2" t="s">
+      <c r="I19" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I19" s="2">
+      <c r="J19" s="2">
         <v>900</v>
       </c>
-      <c r="J19" s="2">
+      <c r="K19" s="2">
         <v>950</v>
       </c>
-      <c r="K19" s="2">
+      <c r="L19" s="2">
         <v>1000</v>
       </c>
-      <c r="L19" s="2">
+      <c r="M19" s="2">
         <v>1050</v>
       </c>
-      <c r="M19" s="2">
+      <c r="N19" s="2">
         <v>1800</v>
       </c>
-      <c r="N19" s="2">
+      <c r="O19" s="2">
         <v>1850</v>
       </c>
-      <c r="O19" s="2">
+      <c r="P19" s="2">
         <v>1900</v>
       </c>
-      <c r="P19" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="Q19" s="2" t="s">
         <v>56</v>
       </c>
       <c r="R19" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="20" spans="1:18" ht="15">
+      <c r="S19" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" ht="15">
       <c r="A20" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B20" s="2">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="C20" s="2">
         <v>4</v>
       </c>
       <c r="D20" s="2">
+        <v>4</v>
+      </c>
+      <c r="E20" s="2">
         <v>19000</v>
       </c>
-      <c r="E20" s="2">
+      <c r="F20" s="2">
         <v>230</v>
       </c>
-      <c r="F20" s="2">
+      <c r="G20" s="2">
         <v>25</v>
       </c>
-      <c r="G20" s="2">
+      <c r="H20" s="2">
         <v>30000</v>
       </c>
-      <c r="H20" s="2" t="s">
+      <c r="I20" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I20" s="2">
+      <c r="J20" s="2">
         <v>950</v>
       </c>
-      <c r="J20" s="2">
+      <c r="K20" s="2">
         <v>1000</v>
       </c>
-      <c r="K20" s="2">
+      <c r="L20" s="2">
         <v>1050</v>
       </c>
-      <c r="L20" s="2">
+      <c r="M20" s="2">
         <v>1100</v>
       </c>
-      <c r="M20" s="2">
+      <c r="N20" s="2">
         <v>1900</v>
       </c>
-      <c r="N20" s="2">
+      <c r="O20" s="2">
         <v>1950</v>
       </c>
-      <c r="O20" s="2">
+      <c r="P20" s="2">
         <v>2000</v>
       </c>
-      <c r="P20" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="Q20" s="2" t="s">
         <v>56</v>
       </c>
       <c r="R20" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="21" spans="1:18" ht="15">
+      <c r="S20" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" ht="15">
       <c r="A21" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B21" s="2">
+        <v>20</v>
+      </c>
+      <c r="C21" s="2">
         <v>4</v>
       </c>
-      <c r="C21" s="2">
+      <c r="D21" s="2">
         <v>5</v>
       </c>
-      <c r="D21" s="2">
+      <c r="E21" s="2">
         <v>20000</v>
       </c>
-      <c r="E21" s="2">
+      <c r="F21" s="2">
         <v>240</v>
       </c>
-      <c r="F21" s="2">
+      <c r="G21" s="2">
         <v>26</v>
       </c>
-      <c r="G21" s="2">
+      <c r="H21" s="2">
         <v>35000</v>
       </c>
-      <c r="H21" s="2" t="s">
+      <c r="I21" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I21" s="2">
+      <c r="J21" s="2">
         <v>1000</v>
       </c>
-      <c r="J21" s="2">
+      <c r="K21" s="2">
         <v>1050</v>
       </c>
-      <c r="K21" s="2">
+      <c r="L21" s="2">
         <v>1100</v>
       </c>
-      <c r="L21" s="2">
+      <c r="M21" s="2">
         <v>1150</v>
       </c>
-      <c r="M21" s="2">
+      <c r="N21" s="2">
         <v>2000</v>
       </c>
-      <c r="N21" s="2">
+      <c r="O21" s="2">
         <v>2050</v>
       </c>
-      <c r="O21" s="2">
+      <c r="P21" s="2">
         <v>2100</v>
       </c>
-      <c r="P21" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="Q21" s="2" t="s">
         <v>56</v>
       </c>
       <c r="R21" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="22" spans="1:18" ht="15">
+      <c r="S21" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" ht="15">
       <c r="A22" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B22" s="2">
+        <v>21</v>
+      </c>
+      <c r="C22" s="2">
         <v>5</v>
       </c>
-      <c r="C22" s="2">
+      <c r="D22" s="2">
         <v>1</v>
       </c>
-      <c r="D22" s="2">
+      <c r="E22" s="2">
         <v>21000</v>
       </c>
-      <c r="E22" s="2">
+      <c r="F22" s="2">
         <v>250</v>
       </c>
-      <c r="F22" s="2">
+      <c r="G22" s="2">
         <v>27</v>
       </c>
-      <c r="G22" s="2">
+      <c r="H22" s="2">
         <v>50000</v>
       </c>
-      <c r="H22" s="2" t="s">
+      <c r="I22" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I22" s="2">
+      <c r="J22" s="2">
         <v>1050</v>
       </c>
-      <c r="J22" s="2">
+      <c r="K22" s="2">
         <v>1100</v>
       </c>
-      <c r="K22" s="2">
+      <c r="L22" s="2">
         <v>1150</v>
       </c>
-      <c r="L22" s="2">
+      <c r="M22" s="2">
         <v>1200</v>
       </c>
-      <c r="M22" s="2">
+      <c r="N22" s="2">
         <v>2100</v>
       </c>
-      <c r="N22" s="2">
+      <c r="O22" s="2">
         <v>2150</v>
       </c>
-      <c r="O22" s="2">
+      <c r="P22" s="2">
         <v>2200</v>
       </c>
-      <c r="P22" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="Q22" s="2" t="s">
         <v>56</v>
       </c>
       <c r="R22" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="23" spans="1:18" ht="15">
+      <c r="S22" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" ht="15">
       <c r="A23" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B23" s="2">
+        <v>22</v>
+      </c>
+      <c r="C23" s="2">
         <v>5</v>
       </c>
-      <c r="C23" s="2">
+      <c r="D23" s="2">
         <v>2</v>
       </c>
-      <c r="D23" s="2">
+      <c r="E23" s="2">
         <v>22000</v>
       </c>
-      <c r="E23" s="2">
+      <c r="F23" s="2">
         <v>260</v>
       </c>
-      <c r="F23" s="2">
+      <c r="G23" s="2">
         <v>28</v>
       </c>
-      <c r="G23" s="2">
+      <c r="H23" s="2">
         <v>55000</v>
       </c>
-      <c r="H23" s="2" t="s">
+      <c r="I23" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I23" s="2">
+      <c r="J23" s="2">
         <v>1100</v>
       </c>
-      <c r="J23" s="2">
+      <c r="K23" s="2">
         <v>1150</v>
       </c>
-      <c r="K23" s="2">
+      <c r="L23" s="2">
         <v>1200</v>
       </c>
-      <c r="L23" s="2">
+      <c r="M23" s="2">
         <v>1250</v>
       </c>
-      <c r="M23" s="2">
+      <c r="N23" s="2">
         <v>2200</v>
       </c>
-      <c r="N23" s="2">
+      <c r="O23" s="2">
         <v>2250</v>
       </c>
-      <c r="O23" s="2">
+      <c r="P23" s="2">
         <v>2300</v>
       </c>
-      <c r="P23" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="Q23" s="2" t="s">
         <v>56</v>
       </c>
       <c r="R23" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="24" spans="1:18" ht="20" customHeight="1">
+      <c r="S23" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" ht="20" customHeight="1">
       <c r="A24" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B24" s="2">
+        <v>23</v>
+      </c>
+      <c r="C24" s="2">
         <v>5</v>
       </c>
-      <c r="C24" s="2">
+      <c r="D24" s="2">
         <v>3</v>
       </c>
-      <c r="D24" s="2">
+      <c r="E24" s="2">
         <v>23000</v>
       </c>
-      <c r="E24" s="2">
+      <c r="F24" s="2">
         <v>270</v>
       </c>
-      <c r="F24" s="2">
+      <c r="G24" s="2">
         <v>29</v>
       </c>
-      <c r="G24" s="2">
+      <c r="H24" s="2">
         <v>60000</v>
       </c>
-      <c r="H24" s="2" t="s">
+      <c r="I24" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I24" s="2">
+      <c r="J24" s="2">
         <v>1150</v>
       </c>
-      <c r="J24" s="2">
+      <c r="K24" s="2">
         <v>1200</v>
       </c>
-      <c r="K24" s="2">
+      <c r="L24" s="2">
         <v>1250</v>
       </c>
-      <c r="L24" s="2">
+      <c r="M24" s="2">
         <v>1300</v>
       </c>
-      <c r="M24" s="2">
+      <c r="N24" s="2">
         <v>2300</v>
       </c>
-      <c r="N24" s="2">
+      <c r="O24" s="2">
         <v>2350</v>
       </c>
-      <c r="O24" s="2">
+      <c r="P24" s="2">
         <v>2400</v>
       </c>
-      <c r="P24" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="Q24" s="2" t="s">
         <v>56</v>
       </c>
       <c r="R24" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="25" spans="1:18" ht="20" customHeight="1">
+      <c r="S24" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" ht="20" customHeight="1">
       <c r="A25" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B25" s="2">
+        <v>24</v>
+      </c>
+      <c r="C25" s="2">
         <v>5</v>
       </c>
-      <c r="C25" s="2">
+      <c r="D25" s="2">
         <v>4</v>
       </c>
-      <c r="D25" s="2">
+      <c r="E25" s="2">
         <v>24000</v>
       </c>
-      <c r="E25" s="2">
+      <c r="F25" s="2">
         <v>280</v>
       </c>
-      <c r="F25" s="2">
+      <c r="G25" s="2">
         <v>30</v>
       </c>
-      <c r="G25" s="2">
+      <c r="H25" s="2">
         <v>65000</v>
       </c>
-      <c r="H25" s="2" t="s">
+      <c r="I25" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I25" s="2">
+      <c r="J25" s="2">
         <v>1200</v>
       </c>
-      <c r="J25" s="2">
+      <c r="K25" s="2">
         <v>1250</v>
       </c>
-      <c r="K25" s="2">
+      <c r="L25" s="2">
         <v>1300</v>
       </c>
-      <c r="L25" s="2">
+      <c r="M25" s="2">
         <v>1350</v>
       </c>
-      <c r="M25" s="2">
+      <c r="N25" s="2">
         <v>2400</v>
       </c>
-      <c r="N25" s="2">
+      <c r="O25" s="2">
         <v>2450</v>
       </c>
-      <c r="O25" s="2">
+      <c r="P25" s="2">
         <v>2500</v>
       </c>
-      <c r="P25" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="Q25" s="2" t="s">
         <v>56</v>
       </c>
       <c r="R25" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="26" spans="1:18" ht="20" customHeight="1">
+      <c r="S25" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" ht="20" customHeight="1">
       <c r="A26" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B26" s="2">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="C26" s="2">
         <v>5</v>
       </c>
       <c r="D26" s="2">
+        <v>5</v>
+      </c>
+      <c r="E26" s="2">
         <v>25000</v>
       </c>
-      <c r="E26" s="2">
+      <c r="F26" s="2">
         <v>290</v>
       </c>
-      <c r="F26" s="2">
+      <c r="G26" s="2">
         <v>31</v>
       </c>
-      <c r="G26" s="2">
+      <c r="H26" s="2">
         <v>70000</v>
       </c>
-      <c r="H26" s="2" t="s">
+      <c r="I26" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I26" s="2">
+      <c r="J26" s="2">
         <v>1250</v>
       </c>
-      <c r="J26" s="2">
+      <c r="K26" s="2">
         <v>1300</v>
       </c>
-      <c r="K26" s="2">
+      <c r="L26" s="2">
         <v>1350</v>
       </c>
-      <c r="L26" s="2">
+      <c r="M26" s="2">
         <v>1400</v>
       </c>
-      <c r="M26" s="2">
+      <c r="N26" s="2">
         <v>2500</v>
       </c>
-      <c r="N26" s="2">
+      <c r="O26" s="2">
         <v>2550</v>
       </c>
-      <c r="O26" s="2">
+      <c r="P26" s="2">
         <v>2600</v>
       </c>
-      <c r="P26" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="Q26" s="2" t="s">
         <v>56</v>
       </c>
       <c r="R26" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="27" spans="1:18" ht="20" customHeight="1">
+      <c r="S26" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" ht="20" customHeight="1">
       <c r="A27" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B27" s="2">
+        <v>26</v>
+      </c>
+      <c r="C27" s="2">
         <v>6</v>
       </c>
-      <c r="C27" s="2">
+      <c r="D27" s="2">
         <v>1</v>
       </c>
-      <c r="D27" s="2">
+      <c r="E27" s="2">
         <v>26000</v>
       </c>
-      <c r="E27" s="2">
+      <c r="F27" s="2">
         <v>300</v>
       </c>
-      <c r="F27" s="2">
+      <c r="G27" s="2">
         <v>32</v>
       </c>
-      <c r="G27" s="2">
+      <c r="H27" s="2">
         <v>100000</v>
       </c>
-      <c r="H27" s="2" t="s">
+      <c r="I27" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I27" s="2">
+      <c r="J27" s="2">
         <v>1300</v>
       </c>
-      <c r="J27" s="2">
+      <c r="K27" s="2">
         <v>1350</v>
       </c>
-      <c r="K27" s="2">
+      <c r="L27" s="2">
         <v>1400</v>
       </c>
-      <c r="L27" s="2">
+      <c r="M27" s="2">
         <v>1450</v>
       </c>
-      <c r="M27" s="2">
+      <c r="N27" s="2">
         <v>2600</v>
       </c>
-      <c r="N27" s="2">
+      <c r="O27" s="2">
         <v>2650</v>
       </c>
-      <c r="O27" s="2">
+      <c r="P27" s="2">
         <v>2700</v>
       </c>
-      <c r="P27" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="Q27" s="2" t="s">
         <v>56</v>
       </c>
       <c r="R27" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="28" spans="1:18" ht="20" customHeight="1">
+      <c r="S27" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" ht="20" customHeight="1">
       <c r="A28" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B28" s="2">
+        <v>27</v>
+      </c>
+      <c r="C28" s="2">
         <v>6</v>
       </c>
-      <c r="C28" s="2">
+      <c r="D28" s="2">
         <v>2</v>
       </c>
-      <c r="D28" s="2">
+      <c r="E28" s="2">
         <v>27000</v>
       </c>
-      <c r="E28" s="2">
+      <c r="F28" s="2">
         <v>310</v>
       </c>
-      <c r="F28" s="2">
+      <c r="G28" s="2">
         <v>33</v>
       </c>
-      <c r="G28" s="2">
+      <c r="H28" s="2">
         <v>150000</v>
       </c>
-      <c r="H28" s="2" t="s">
+      <c r="I28" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I28" s="2">
+      <c r="J28" s="2">
         <v>1350</v>
       </c>
-      <c r="J28" s="2">
+      <c r="K28" s="2">
         <v>1400</v>
       </c>
-      <c r="K28" s="2">
+      <c r="L28" s="2">
         <v>1450</v>
       </c>
-      <c r="L28" s="2">
+      <c r="M28" s="2">
         <v>1500</v>
       </c>
-      <c r="M28" s="2">
+      <c r="N28" s="2">
         <v>2700</v>
       </c>
-      <c r="N28" s="2">
+      <c r="O28" s="2">
         <v>2750</v>
       </c>
-      <c r="O28" s="2">
+      <c r="P28" s="2">
         <v>2800</v>
       </c>
-      <c r="P28" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="Q28" s="2" t="s">
         <v>56</v>
       </c>
       <c r="R28" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="29" spans="1:18" ht="20" customHeight="1">
+      <c r="S28" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" ht="20" customHeight="1">
       <c r="A29" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B29" s="2">
+        <v>28</v>
+      </c>
+      <c r="C29" s="2">
         <v>6</v>
       </c>
-      <c r="C29" s="2">
+      <c r="D29" s="2">
         <v>3</v>
       </c>
-      <c r="D29" s="2">
+      <c r="E29" s="2">
         <v>28000</v>
       </c>
-      <c r="E29" s="2">
+      <c r="F29" s="2">
         <v>320</v>
       </c>
-      <c r="F29" s="2">
+      <c r="G29" s="2">
         <v>34</v>
       </c>
-      <c r="G29" s="2">
+      <c r="H29" s="2">
         <v>200000</v>
       </c>
-      <c r="H29" s="2" t="s">
+      <c r="I29" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I29" s="2">
+      <c r="J29" s="2">
         <v>1400</v>
       </c>
-      <c r="J29" s="2">
+      <c r="K29" s="2">
         <v>1450</v>
       </c>
-      <c r="K29" s="2">
+      <c r="L29" s="2">
         <v>1500</v>
       </c>
-      <c r="L29" s="2">
+      <c r="M29" s="2">
         <v>1550</v>
       </c>
-      <c r="M29" s="2">
+      <c r="N29" s="2">
         <v>2800</v>
       </c>
-      <c r="N29" s="2">
+      <c r="O29" s="2">
         <v>2850</v>
       </c>
-      <c r="O29" s="2">
+      <c r="P29" s="2">
         <v>2900</v>
       </c>
-      <c r="P29" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="Q29" s="2" t="s">
         <v>56</v>
       </c>
       <c r="R29" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="30" spans="1:18" ht="20" customHeight="1">
+      <c r="S29" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" ht="20" customHeight="1">
       <c r="A30" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B30" s="2">
+        <v>29</v>
+      </c>
+      <c r="C30" s="2">
         <v>6</v>
       </c>
-      <c r="C30" s="2">
+      <c r="D30" s="2">
         <v>4</v>
       </c>
-      <c r="D30" s="2">
+      <c r="E30" s="2">
         <v>29000</v>
       </c>
-      <c r="E30" s="2">
+      <c r="F30" s="2">
         <v>330</v>
       </c>
-      <c r="F30" s="2">
+      <c r="G30" s="2">
         <v>35</v>
       </c>
-      <c r="G30" s="2">
+      <c r="H30" s="2">
         <v>250000</v>
       </c>
-      <c r="H30" s="2" t="s">
+      <c r="I30" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I30" s="2">
+      <c r="J30" s="2">
         <v>1450</v>
       </c>
-      <c r="J30" s="2">
+      <c r="K30" s="2">
         <v>1500</v>
       </c>
-      <c r="K30" s="2">
+      <c r="L30" s="2">
         <v>1550</v>
       </c>
-      <c r="L30" s="2">
+      <c r="M30" s="2">
         <v>1600</v>
       </c>
-      <c r="M30" s="2">
+      <c r="N30" s="2">
         <v>2900</v>
       </c>
-      <c r="N30" s="2">
+      <c r="O30" s="2">
         <v>2950</v>
       </c>
-      <c r="O30" s="2">
+      <c r="P30" s="2">
         <v>3000</v>
       </c>
-      <c r="P30" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="Q30" s="2" t="s">
         <v>56</v>
       </c>
       <c r="R30" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="31" spans="1:18" ht="20" customHeight="1">
+      <c r="S30" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" ht="20" customHeight="1">
       <c r="A31" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B31" s="2">
+        <v>30</v>
+      </c>
+      <c r="C31" s="2">
         <v>6</v>
       </c>
-      <c r="C31" s="2">
+      <c r="D31" s="2">
         <v>5</v>
       </c>
-      <c r="D31" s="2">
+      <c r="E31" s="2">
         <v>30000</v>
       </c>
-      <c r="E31" s="2">
+      <c r="F31" s="2">
         <v>340</v>
       </c>
-      <c r="F31" s="2">
+      <c r="G31" s="2">
         <v>36</v>
       </c>
-      <c r="G31" s="2">
+      <c r="H31" s="2">
         <v>300000</v>
       </c>
-      <c r="H31" s="2" t="s">
+      <c r="I31" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I31" s="2">
+      <c r="J31" s="2">
         <v>1500</v>
       </c>
-      <c r="J31" s="2">
+      <c r="K31" s="2">
         <v>1550</v>
       </c>
-      <c r="K31" s="2">
+      <c r="L31" s="2">
         <v>1600</v>
       </c>
-      <c r="L31" s="2">
+      <c r="M31" s="2">
         <v>1650</v>
       </c>
-      <c r="M31" s="2">
+      <c r="N31" s="2">
         <v>3000</v>
       </c>
-      <c r="N31" s="2">
+      <c r="O31" s="2">
         <v>3050</v>
       </c>
-      <c r="O31" s="2">
+      <c r="P31" s="2">
         <v>3100</v>
       </c>
-      <c r="P31" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="Q31" s="2" t="s">
         <v>56</v>
       </c>
       <c r="R31" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="S31" s="2" t="s">
         <v>56</v>
       </c>
     </row>

</xml_diff>

<commit_message>
dev of alliance village
</commit_message>
<xml_diff>
--- a/gameData/shared/AllianceShrine.xlsx
+++ b/gameData/shared/AllianceShrine.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7460" yWindow="1780" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="7080" yWindow="2040" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="shrineStage" sheetId="4" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="52">
   <si>
     <t>INT_suggestPlayer</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -168,30 +168,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>swordsman_1:10,sentinel_1:10,ranger_1:10&amp;swordsman_1:10,sentinel_1:10,ranger_1:10</t>
-  </si>
-  <si>
-    <t>swordsman_1:12,sentinel_1:12,ranger_1:12&amp;swordsman_1:12,sentinel_1:12,ranger_1:12</t>
-  </si>
-  <si>
-    <t>swordsman_1:14,sentinel_1:14,ranger_1:14&amp;swordsman_1:14,sentinel_1:14,ranger_1:14</t>
-  </si>
-  <si>
-    <t>swordsman_1:16,sentinel_1:16,ranger_1:16&amp;swordsman_1:16,sentinel_1:10,ranger_1:16</t>
-  </si>
-  <si>
-    <t>swordsman_1:18,sentinel_1:18,ranger_1:18&amp;swordsman_1:18,sentinel_1:18,ranger_1:18</t>
-  </si>
-  <si>
-    <t>swordsman_1:22,sentinel_1:22,ranger_1:22&amp;swordsman_1:22,sentinel_1:22,ranger_1:22</t>
-  </si>
-  <si>
-    <t>swordsman_1:24,sentinel_1:24,ranger_1:24&amp;swordsman_1:24,sentinel_1:24,ranger_1:24</t>
-  </si>
-  <si>
-    <t>swordsman_1:20,sentinel_1:20,ranger_1:20&amp;swordsman_1:20,sentinel_1:20,ranger_1:20</t>
-  </si>
-  <si>
     <t>INT_star3Honour</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -217,10 +193,6 @@
   </si>
   <si>
     <t>STR_goldRewards</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>swordsman_1:10,sentinel_1:10,ranger_1:10&amp;swordsman_1:10,sentinel_1:10,ranger_1:10</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -237,6 +209,10 @@
   <si>
     <t>INT_index</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>redDragon_1_5,swordsman_1_10,sentinel_1_10,ranger_1_10&amp;swordsman_1_10,sentinel_1_10,ranger_1_10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -322,8 +298,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="129">
+  <cellStyleXfs count="135">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -462,7 +444,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="129">
+  <cellStyles count="135">
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
@@ -527,6 +509,9 @@
     <cellStyle name="超链接" xfId="123" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="125" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="133" builtinId="8" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
@@ -591,6 +576,9 @@
     <cellStyle name="访问过的超链接" xfId="124" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="126" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="134" builtinId="9" hidden="1"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -922,8 +910,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S31"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -940,7 +928,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>4</v>
@@ -964,7 +952,7 @@
         <v>39</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>37</v>
@@ -973,25 +961,25 @@
         <v>38</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="15">
@@ -1020,7 +1008,7 @@
         <v>350</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="J2" s="2">
         <v>50</v>
@@ -1044,13 +1032,13 @@
         <v>20</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="15">
@@ -1079,7 +1067,7 @@
         <v>400</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="J3" s="2">
         <v>100</v>
@@ -1103,13 +1091,13 @@
         <v>300</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="15">
@@ -1138,7 +1126,7 @@
         <v>450</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="J4" s="2">
         <v>150</v>
@@ -1162,13 +1150,13 @@
         <v>400</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="S4" s="2" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:19" ht="15">
@@ -1197,7 +1185,7 @@
         <v>500</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="J5" s="2">
         <v>200</v>
@@ -1221,13 +1209,13 @@
         <v>500</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="S5" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="15">
@@ -1256,7 +1244,7 @@
         <v>1000</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="J6" s="2">
         <v>250</v>
@@ -1280,13 +1268,13 @@
         <v>600</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="S6" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="15">
@@ -1315,7 +1303,7 @@
         <v>2000</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="J7" s="2">
         <v>300</v>
@@ -1339,13 +1327,13 @@
         <v>700</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="S7" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="15">
@@ -1374,7 +1362,7 @@
         <v>2500</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="J8" s="2">
         <v>350</v>
@@ -1398,13 +1386,13 @@
         <v>800</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="R8" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="S8" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:19" ht="15">
@@ -1433,7 +1421,7 @@
         <v>3000</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="J9" s="2">
         <v>400</v>
@@ -1457,13 +1445,13 @@
         <v>900</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="R9" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="S9" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:19" ht="15">
@@ -1492,7 +1480,7 @@
         <v>3500</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="J10" s="2">
         <v>450</v>
@@ -1516,13 +1504,13 @@
         <v>1000</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="R10" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="S10" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:19" ht="15">
@@ -1551,7 +1539,7 @@
         <v>4000</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="J11" s="2">
         <v>500</v>
@@ -1575,13 +1563,13 @@
         <v>1100</v>
       </c>
       <c r="Q11" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="R11" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="S11" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:19" ht="15">
@@ -1610,7 +1598,7 @@
         <v>5000</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="J12" s="2">
         <v>550</v>
@@ -1634,13 +1622,13 @@
         <v>1200</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="R12" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="S12" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:19" ht="15">
@@ -1669,7 +1657,7 @@
         <v>6000</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="J13" s="2">
         <v>600</v>
@@ -1693,13 +1681,13 @@
         <v>1300</v>
       </c>
       <c r="Q13" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="R13" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="S13" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:19" ht="15">
@@ -1728,7 +1716,7 @@
         <v>7000</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="J14" s="2">
         <v>650</v>
@@ -1752,13 +1740,13 @@
         <v>1400</v>
       </c>
       <c r="Q14" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="R14" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="S14" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:19" ht="15">
@@ -1787,7 +1775,7 @@
         <v>8000</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="J15" s="2">
         <v>700</v>
@@ -1811,13 +1799,13 @@
         <v>1500</v>
       </c>
       <c r="Q15" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="R15" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="S15" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:19" ht="15">
@@ -1846,7 +1834,7 @@
         <v>10000</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="J16" s="2">
         <v>750</v>
@@ -1870,13 +1858,13 @@
         <v>1600</v>
       </c>
       <c r="Q16" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="R16" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="S16" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:19" ht="15">
@@ -1905,7 +1893,7 @@
         <v>15000</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="J17" s="2">
         <v>800</v>
@@ -1929,13 +1917,13 @@
         <v>1700</v>
       </c>
       <c r="Q17" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="R17" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="S17" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:19" ht="15">
@@ -1964,7 +1952,7 @@
         <v>20000</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="J18" s="2">
         <v>850</v>
@@ -1988,13 +1976,13 @@
         <v>1800</v>
       </c>
       <c r="Q18" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="R18" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="S18" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:19" ht="15">
@@ -2023,7 +2011,7 @@
         <v>25000</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="J19" s="2">
         <v>900</v>
@@ -2047,13 +2035,13 @@
         <v>1900</v>
       </c>
       <c r="Q19" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="R19" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="S19" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:19" ht="15">
@@ -2082,7 +2070,7 @@
         <v>30000</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="J20" s="2">
         <v>950</v>
@@ -2106,13 +2094,13 @@
         <v>2000</v>
       </c>
       <c r="Q20" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="R20" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="S20" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:19" ht="15">
@@ -2141,7 +2129,7 @@
         <v>35000</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="J21" s="2">
         <v>1000</v>
@@ -2165,13 +2153,13 @@
         <v>2100</v>
       </c>
       <c r="Q21" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="R21" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="S21" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:19" ht="15">
@@ -2200,7 +2188,7 @@
         <v>50000</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="J22" s="2">
         <v>1050</v>
@@ -2224,13 +2212,13 @@
         <v>2200</v>
       </c>
       <c r="Q22" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="R22" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="S22" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:19" ht="15">
@@ -2259,7 +2247,7 @@
         <v>55000</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="J23" s="2">
         <v>1100</v>
@@ -2283,13 +2271,13 @@
         <v>2300</v>
       </c>
       <c r="Q23" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="R23" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="S23" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:19" ht="20" customHeight="1">
@@ -2318,7 +2306,7 @@
         <v>60000</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="J24" s="2">
         <v>1150</v>
@@ -2342,13 +2330,13 @@
         <v>2400</v>
       </c>
       <c r="Q24" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="R24" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="S24" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:19" ht="20" customHeight="1">
@@ -2377,7 +2365,7 @@
         <v>65000</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="J25" s="2">
         <v>1200</v>
@@ -2401,13 +2389,13 @@
         <v>2500</v>
       </c>
       <c r="Q25" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="R25" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="S25" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:19" ht="20" customHeight="1">
@@ -2436,7 +2424,7 @@
         <v>70000</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="J26" s="2">
         <v>1250</v>
@@ -2460,13 +2448,13 @@
         <v>2600</v>
       </c>
       <c r="Q26" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="R26" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="S26" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="1:19" ht="20" customHeight="1">
@@ -2495,7 +2483,7 @@
         <v>100000</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="J27" s="2">
         <v>1300</v>
@@ -2519,13 +2507,13 @@
         <v>2700</v>
       </c>
       <c r="Q27" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="R27" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="S27" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
     </row>
     <row r="28" spans="1:19" ht="20" customHeight="1">
@@ -2554,7 +2542,7 @@
         <v>150000</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="J28" s="2">
         <v>1350</v>
@@ -2578,13 +2566,13 @@
         <v>2800</v>
       </c>
       <c r="Q28" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="R28" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="S28" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:19" ht="20" customHeight="1">
@@ -2613,7 +2601,7 @@
         <v>200000</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="J29" s="2">
         <v>1400</v>
@@ -2637,13 +2625,13 @@
         <v>2900</v>
       </c>
       <c r="Q29" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="R29" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="S29" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:19" ht="20" customHeight="1">
@@ -2672,7 +2660,7 @@
         <v>250000</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="J30" s="2">
         <v>1450</v>
@@ -2696,13 +2684,13 @@
         <v>3000</v>
       </c>
       <c r="Q30" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="R30" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="S30" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
     </row>
     <row r="31" spans="1:19" ht="20" customHeight="1">
@@ -2731,7 +2719,7 @@
         <v>300000</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="J31" s="2">
         <v>1500</v>
@@ -2755,13 +2743,13 @@
         <v>3100</v>
       </c>
       <c r="Q31" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="R31" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="S31" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>